<commit_message>
Added placebombcommand and tried to make a bombcomponent
changed the level slightly
</commit_message>
<xml_diff>
--- a/Data/levels/LevelLayout1.xlsx
+++ b/Data/levels/LevelLayout1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\howest\2023-2024\prog4\2DAE19_Delie_Wout_exam\bigigin\Data\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72958A52-9E0F-4945-B013-AC41F2BD3FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C458E1-241A-4083-986A-3011C484991B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{3EF8BAA1-4477-4F67-8127-E5218CC04581}"/>
   </bookViews>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CCF307-98E7-492C-B514-DC0B2B2F3D5E}">
   <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:AD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,13 +527,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -545,13 +545,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
       </c>
       <c r="K2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -560,13 +560,13 @@
         <v>1</v>
       </c>
       <c r="N2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
       </c>
       <c r="P2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="2">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="X2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" s="2">
         <v>1</v>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -717,13 +717,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
@@ -744,25 +744,25 @@
         <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="2">
         <v>1</v>
       </c>
       <c r="N4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4" s="2">
         <v>1</v>
       </c>
       <c r="P4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="2">
         <v>1</v>
       </c>
       <c r="R4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S4" s="2">
         <v>1</v>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="V4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W4" s="2">
         <v>1</v>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="Z4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="2">
         <v>1</v>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="AD4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE4" s="1">
         <v>0</v>
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -863,19 +863,19 @@
         <v>0</v>
       </c>
       <c r="T5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -922,19 +922,19 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="2">
         <v>1</v>
@@ -943,34 +943,34 @@
         <v>1</v>
       </c>
       <c r="O6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="2">
         <v>1</v>
       </c>
       <c r="R6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6" s="2">
         <v>1</v>
       </c>
       <c r="V6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="2">
         <v>1</v>
@@ -982,13 +982,13 @@
         <v>1</v>
       </c>
       <c r="AB6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC6" s="2">
         <v>1</v>
       </c>
       <c r="AD6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE6" s="1">
         <v>0</v>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -1059,19 +1059,19 @@
         <v>0</v>
       </c>
       <c r="V7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y7">
         <v>0</v>
       </c>
       <c r="Z7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -1094,19 +1094,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
@@ -1130,13 +1130,13 @@
         <v>1</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="2">
         <v>1</v>
       </c>
       <c r="P8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="2">
         <v>1</v>
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W8" s="2">
         <v>1</v>
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="Z8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA8" s="2">
         <v>1</v>
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="AC8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD8" s="2">
         <v>1</v>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1249,13 +1249,13 @@
         <v>0</v>
       </c>
       <c r="V9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1284,91 +1284,91 @@
         <v>0</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="2">
         <v>1</v>
       </c>
       <c r="S10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U10" s="2">
         <v>1</v>
       </c>
       <c r="V10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE10" s="1">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1486,13 +1486,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -1504,25 +1504,25 @@
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12" s="2">
         <v>1</v>
       </c>
       <c r="P12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="2">
         <v>1</v>
       </c>
       <c r="R12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="U12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12" s="2">
         <v>1</v>

</xml_diff>